<commit_message>
Added deensity step size option
</commit_message>
<xml_diff>
--- a/Planilhas de análise/Envelope_plot.xlsx
+++ b/Planilhas de análise/Envelope_plot.xlsx
@@ -864,178 +864,133 @@
                   <c:v>5.8591042637381996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4831424502627097</c:v>
+                  <c:v>7.3018891515019302</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4611222799053003</c:v>
+                  <c:v>7.2766672008740603</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4388143614602802</c:v>
+                  <c:v>7.2512626345506597</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.41630016041786</c:v>
+                  <c:v>7.2255672912393996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.3936968588212304</c:v>
+                  <c:v>7.1994684442101198</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3707901607294604</c:v>
+                  <c:v>7.1731400810556103</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3476746441518497</c:v>
+                  <c:v>7.1464790066373496</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.3244412252413902</c:v>
+                  <c:v>7.1193850451695502</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.3008816821148601</c:v>
+                  <c:v>7.0920333311784196</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.27709836821181</c:v>
+                  <c:v>7.0642999904731596</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.2531813195828603</c:v>
+                  <c:v>7.0361768613322502</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.2289090372456997</c:v>
+                  <c:v>7.0076464721156997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.2044943211291796</c:v>
+                  <c:v>6.9786894935616903</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.1797101657913496</c:v>
+                  <c:v>6.94927443655574</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.1547782843857899</c:v>
+                  <c:v>6.9194854421776597</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.1294471958867396</c:v>
+                  <c:v>6.8891167800800996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.1039347709624598</c:v>
+                  <c:v>6.8582230834512101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.0780099392793696</c:v>
+                  <c:v>6.82685144210192</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.0518882533204499</c:v>
+                  <c:v>6.7948152129236501</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.0253397060208798</c:v>
+                  <c:v>6.76224572120225</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.9985578180577601</c:v>
+                  <c:v>6.7289937059384597</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.9714204339209003</c:v>
+                  <c:v>6.6950438339079597</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.9439131958592304</c:v>
+                  <c:v>6.6604192436680902</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.9159019831246802</c:v>
+                  <c:v>6.6248628520981301</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.8876090933653904</c:v>
+                  <c:v>6.58852417074442</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.8588917375556901</c:v>
+                  <c:v>6.55119306636694</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.8297287323044502</c:v>
+                  <c:v>6.5129203956428299</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.8001270657856798</c:v>
+                  <c:v>6.47339369910532</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.7700018202915802</c:v>
+                  <c:v>6.43276529681975</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.7394769323194703</c:v>
+                  <c:v>6.3906744816543402</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.7082793330174697</c:v>
+                  <c:v>6.3470732133511198</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.6765942738238504</c:v>
+                  <c:v>6.3017796878727799</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.6441820109603702</c:v>
+                  <c:v>6.2544678428308504</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.6112217940153597</c:v>
+                  <c:v>6.2049688977114403</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.5775455297792398</c:v>
+                  <c:v>6.1526786449464304</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.5431011109783697</c:v>
+                  <c:v>6.0973673724428501</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6.5077401965147601</c:v>
+                  <c:v>6.03810345559108</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.4716884292177204</c:v>
+                  <c:v>5.9742055756659802</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.4346555663204601</c:v>
+                  <c:v>5.90414454234367</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.3965538532516897</c:v>
+                  <c:v>5.8252621445605497</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.3573667733563202</c:v>
+                  <c:v>5.7329821766848204</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.3169155565285697</c:v>
+                  <c:v>5.6322921702051296</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.2749825629684697</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.23156863249437</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.1865116347403202</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.1393419397654503</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6.0900581556244102</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.0378291254429799</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.98253987504809</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.9232941847193104</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.8591042637475397</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.7883374475500702</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5.7082043904962498</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.6144136809769902</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.5256936776569301</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.3835194730617904</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.2189926932794002</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.1767006727176001</c:v>
+                  <c:v>5.5101642502389296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1077,178 +1032,133 @@
                   <c:v>42.460082772624403</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.642891981919497</c:v>
+                  <c:v>34.842352620883197</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.784199883701902</c:v>
+                  <c:v>34.987904494824903</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.925265348824603</c:v>
+                  <c:v>35.134884796496003</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.066838561414599</c:v>
+                  <c:v>35.2826385485956</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.209888874959397</c:v>
+                  <c:v>35.430556350401503</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35.352761955459599</c:v>
+                  <c:v>35.579778826172401</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.496265793378299</c:v>
+                  <c:v>35.729750281573203</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35.641112056516498</c:v>
+                  <c:v>35.880002453428098</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.785811733904502</c:v>
+                  <c:v>36.031590582370498</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35.931183106709703</c:v>
+                  <c:v>36.183911866677398</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.077885756664401</c:v>
+                  <c:v>36.337016036260898</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.224453189127303</c:v>
+                  <c:v>36.490910092770299</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.372370647484203</c:v>
+                  <c:v>36.645598689250903</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.520211105239099</c:v>
+                  <c:v>36.8010385713213</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.669444275542602</c:v>
+                  <c:v>36.957695757109299</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.8185719294652</c:v>
+                  <c:v>37.1147844590392</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.968975569694699</c:v>
+                  <c:v>37.272672366635497</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>37.1193672660972</c:v>
+                  <c:v>37.431653607261602</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>37.271042590135202</c:v>
+                  <c:v>37.591141466962597</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37.4227972824131</c:v>
+                  <c:v>37.751754258756499</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>37.575742591242097</c:v>
+                  <c:v>37.9130954060061</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>37.729294141154803</c:v>
+                  <c:v>38.075269858279697</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37.8834615702809</c:v>
+                  <c:v>38.238492347002399</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>38.037703004000797</c:v>
+                  <c:v>38.402167553409697</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>38.193151274937797</c:v>
+                  <c:v>38.5669154842643</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38.349218575694401</c:v>
+                  <c:v>38.732354549600601</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>38.505906597864801</c:v>
+                  <c:v>38.898817671040597</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38.663338174684498</c:v>
+                  <c:v>39.0657974707675</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.821272323558503</c:v>
+                  <c:v>39.233884301274202</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>38.980281154274998</c:v>
+                  <c:v>39.402592713501903</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>39.139455669267797</c:v>
+                  <c:v>39.572149149139697</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>39.299589815164197</c:v>
+                  <c:v>39.742558688364497</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>39.459989326798699</c:v>
+                  <c:v>39.913676150553897</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>39.621377507594303</c:v>
+                  <c:v>40.085682094038503</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>39.783348209641701</c:v>
+                  <c:v>40.258288120218502</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>39.945904411970801</c:v>
+                  <c:v>40.431814431181699</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>40.108815865754202</c:v>
+                  <c:v>40.605990010074798</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>40.272843546997301</c:v>
+                  <c:v>40.781058709310898</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>40.437406489114998</c:v>
+                  <c:v>40.956904102251102</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>40.602513182169197</c:v>
+                  <c:v>41.133366215811698</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>40.768344322168197</c:v>
+                  <c:v>41.310479629077903</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>40.934759430510603</c:v>
+                  <c:v>41.491122903159997</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41.101624535925801</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>41.269240846022903</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>41.437629944779196</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>41.606451722751601</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>41.776113552696302</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>41.946084886906696</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>42.116833187358097</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>42.288155040503298</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>42.4600827726075</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>42.632579463731503</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>42.805605187939598</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>42.979457979611098</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43.158833678275698</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43.333919633036402</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43.509159976231501</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>43.684236904605399</c:v>
+                  <c:v>41.6726240396601</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1322,178 +1232,133 @@
                   <c:v>4.4264075542562802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6563626323753802</c:v>
+                  <c:v>2.8531002316127001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.6789998652238398</c:v>
+                  <c:v>2.8824543798668101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7020347861968199</c:v>
+                  <c:v>2.91213927462955</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.72540193146085</c:v>
+                  <c:v>2.9423658895290199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7489993608392398</c:v>
+                  <c:v>2.97335045770313</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7730144403683799</c:v>
+                  <c:v>3.0047089993527498</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.79737648471309</c:v>
+                  <c:v>3.0366480477145501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8219815775772101</c:v>
+                  <c:v>3.06938835049734</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.8470395677946398</c:v>
+                  <c:v>3.1025302345000401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8724556087081199</c:v>
+                  <c:v>3.1362624263021202</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.8981154434937402</c:v>
+                  <c:v>3.1706156802835901</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.9242663966509999</c:v>
+                  <c:v>3.2056011295691</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.9506652454842599</c:v>
+                  <c:v>3.24123099886905</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9775727572095398</c:v>
+                  <c:v>3.2775765627748501</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.00472762254245</c:v>
+                  <c:v>3.3142994248016402</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.03242028518746</c:v>
+                  <c:v>3.3519458315863702</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0603765933872298</c:v>
+                  <c:v>3.3903018857585399</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.0888913712488701</c:v>
+                  <c:v>3.4292123098740999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.11767251432993</c:v>
+                  <c:v>3.46905176295492</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1470352401498198</c:v>
+                  <c:v>3.5094150983626702</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1766798277811499</c:v>
+                  <c:v>3.5506792187559699</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.2067775022090101</c:v>
+                  <c:v>3.5926997823234199</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2373386829415698</c:v>
+                  <c:v>3.6353685629694699</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2685488238789699</c:v>
+                  <c:v>3.6793127638147198</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3000717155730999</c:v>
+                  <c:v>3.7239086094375602</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.3321013288048702</c:v>
+                  <c:v>3.76969783538929</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3646548282586002</c:v>
+                  <c:v>3.8162745603866499</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3977296008513602</c:v>
+                  <c:v>3.8643092047473102</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.4313901570629701</c:v>
+                  <c:v>3.91327673162627</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.4654524094832899</c:v>
+                  <c:v>3.9639220053655402</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.50031049286109</c:v>
+                  <c:v>4.0160633169199</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.5356896644051399</c:v>
+                  <c:v>4.0695741153676801</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.5718766570333802</c:v>
+                  <c:v>4.1253983256757802</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.6085955970210599</c:v>
+                  <c:v>4.1831517733499304</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.6460762289934201</c:v>
+                  <c:v>4.2437064262652697</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.6843655108036999</c:v>
+                  <c:v>4.30711417948143</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.7236478087345599</c:v>
+                  <c:v>4.3743908476388302</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.7635569050858999</c:v>
+                  <c:v>4.44648047249082</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.80447931122325</c:v>
+                  <c:v>4.5248235803186203</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.84649617019529</c:v>
+                  <c:v>4.6111301540093601</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.8896589765555301</c:v>
+                  <c:v>4.7097269013225596</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.93402918314922</c:v>
+                  <c:v>4.8005269780342301</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.97991302157924</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4.02723884162</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4.07629253628272</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4.1272113050055204</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4.1804769580021004</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4.2363421539307202</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4.2953649712256299</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.3585978267418799</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4.4264075542626404</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4.5005994716257698</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>4.5835983449190403</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4.6816306404680699</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>4.7692325677298504</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>4.9164465213469697</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.0798197261805598</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.1187358618182</c:v>
+                  <c:v>4.9441771534810304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1535,178 +1400,133 @@
                   <c:v>42.464911071650803</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.645889337403403</c:v>
+                  <c:v>34.845015308570296</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.786376833659403</c:v>
+                  <c:v>34.991311900615102</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.927730029337397</c:v>
+                  <c:v>35.137899592907701</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.0697295457013</c:v>
+                  <c:v>35.2852647153235</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>35.2120641713786</c:v>
+                  <c:v>35.433863707544603</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>35.3552753934949</c:v>
+                  <c:v>35.582836097645497</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.499138819707902</c:v>
+                  <c:v>35.732625826480302</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35.643351734063103</c:v>
+                  <c:v>35.8836662525881</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.788489989048003</c:v>
+                  <c:v>36.035120585260998</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35.9342722821672</c:v>
+                  <c:v>36.187367381036204</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.0803820558084</c:v>
+                  <c:v>36.340452021841401</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.227466030799498</c:v>
+                  <c:v>36.494378735286602</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.374872127760497</c:v>
+                  <c:v>36.649152049319603</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.523257237233501</c:v>
+                  <c:v>36.804877522812397</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.671946578979203</c:v>
+                  <c:v>36.960951355264498</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.821644025351901</c:v>
+                  <c:v>37.118294283752597</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.971666514505799</c:v>
+                  <c:v>37.276503998255897</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>37.122697602738803</c:v>
+                  <c:v>37.435308216641403</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>37.274038150082802</c:v>
+                  <c:v>37.595265087267002</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>37.426388292401697</c:v>
+                  <c:v>37.755717475365202</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>37.579056274961196</c:v>
+                  <c:v>37.917193404168003</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>37.732406006891303</c:v>
+                  <c:v>38.079432357345098</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>37.886435001704797</c:v>
+                  <c:v>38.242247831969699</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>38.041493153379101</c:v>
+                  <c:v>38.406412639390297</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>38.196863220224401</c:v>
+                  <c:v>38.571038054832798</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>38.352915402140503</c:v>
+                  <c:v>38.736731430078102</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>38.5096496517994</c:v>
+                  <c:v>38.9029207134651</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>38.667026038769897</c:v>
+                  <c:v>39.070276489066103</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>38.825124636515802</c:v>
+                  <c:v>39.238103862201399</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>38.983581340417302</c:v>
+                  <c:v>39.407053578167101</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>39.143042722784301</c:v>
+                  <c:v>39.576767992627303</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>39.302983085392</c:v>
+                  <c:v>39.746980567877699</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>39.463821025764197</c:v>
+                  <c:v>39.918315466547902</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>39.625054928453999</c:v>
+                  <c:v>40.090203719673703</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>39.786988246620702</c:v>
+                  <c:v>40.263029947619202</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>39.949616136718397</c:v>
+                  <c:v>40.436481331258499</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>40.113112293822901</c:v>
+                  <c:v>40.610783840922203</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>40.2768871016278</c:v>
+                  <c:v>40.785903072507899</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>40.441381504629703</c:v>
+                  <c:v>40.961810241869102</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>40.606584340992796</c:v>
+                  <c:v>41.138274168016103</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>40.772434626252199</c:v>
+                  <c:v>41.3154075510176</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>40.938873788102299</c:v>
+                  <c:v>41.488676211309603</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>41.106082816166101</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>41.273812097923503</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>41.442158170747703</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>41.611033233424301</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>41.780590537770898</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>41.950717442605701</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>42.121449536862599</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>42.2929730689198</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>42.464911071649396</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>42.637431668547499</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>42.810497148708997</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>42.984416209589</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>43.153859152428701</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>43.328927528517802</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43.504161769781497</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>43.6792386926479</c:v>
+                  <c:v>41.667632393692898</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11418,178 +11238,133 @@
                   <c:v>5.8591042637381996</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.4831424502627097</c:v>
+                  <c:v>7.3018891515019302</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>7.4611222799053003</c:v>
+                  <c:v>7.2766672008740603</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.4388143614602802</c:v>
+                  <c:v>7.2512626345506597</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>7.41630016041786</c:v>
+                  <c:v>7.2255672912393996</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>7.3936968588212304</c:v>
+                  <c:v>7.1994684442101198</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.3707901607294604</c:v>
+                  <c:v>7.1731400810556103</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3476746441518497</c:v>
+                  <c:v>7.1464790066373496</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.3244412252413902</c:v>
+                  <c:v>7.1193850451695502</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.3008816821148601</c:v>
+                  <c:v>7.0920333311784196</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.27709836821181</c:v>
+                  <c:v>7.0642999904731596</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>7.2531813195828603</c:v>
+                  <c:v>7.0361768613322502</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>7.2289090372456997</c:v>
+                  <c:v>7.0076464721156997</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.2044943211291796</c:v>
+                  <c:v>6.9786894935616903</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.1797101657913496</c:v>
+                  <c:v>6.94927443655574</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.1547782843857899</c:v>
+                  <c:v>6.9194854421776597</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.1294471958867396</c:v>
+                  <c:v>6.8891167800800996</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>7.1039347709624598</c:v>
+                  <c:v>6.8582230834512101</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>7.0780099392793696</c:v>
+                  <c:v>6.82685144210192</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.0518882533204499</c:v>
+                  <c:v>6.7948152129236501</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.0253397060208798</c:v>
+                  <c:v>6.76224572120225</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.9985578180577601</c:v>
+                  <c:v>6.7289937059384597</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.9714204339209003</c:v>
+                  <c:v>6.6950438339079597</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>6.9439131958592304</c:v>
+                  <c:v>6.6604192436680902</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.9159019831246802</c:v>
+                  <c:v>6.6248628520981301</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>6.8876090933653904</c:v>
+                  <c:v>6.58852417074442</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.8588917375556901</c:v>
+                  <c:v>6.55119306636694</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>6.8297287323044502</c:v>
+                  <c:v>6.5129203956428299</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.8001270657856798</c:v>
+                  <c:v>6.47339369910532</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>6.7700018202915802</c:v>
+                  <c:v>6.43276529681975</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>6.7394769323194703</c:v>
+                  <c:v>6.3906744816543402</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>6.7082793330174697</c:v>
+                  <c:v>6.3470732133511198</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>6.6765942738238504</c:v>
+                  <c:v>6.3017796878727799</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.6441820109603702</c:v>
+                  <c:v>6.2544678428308504</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.6112217940153597</c:v>
+                  <c:v>6.2049688977114403</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>6.5775455297792398</c:v>
+                  <c:v>6.1526786449464304</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>6.5431011109783697</c:v>
+                  <c:v>6.0973673724428501</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>6.5077401965147601</c:v>
+                  <c:v>6.03810345559108</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>6.4716884292177204</c:v>
+                  <c:v>5.9742055756659802</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>6.4346555663204601</c:v>
+                  <c:v>5.90414454234367</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>6.3965538532516897</c:v>
+                  <c:v>5.8252621445605497</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>6.3573667733563202</c:v>
+                  <c:v>5.7329821766848204</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>6.3169155565285697</c:v>
+                  <c:v>5.6322921702051296</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>6.2749825629684697</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>6.23156863249437</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.1865116347403202</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>6.1393419397654503</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>6.0900581556244102</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>6.0378291254429799</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>5.98253987504809</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>5.9232941847193104</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>5.8591042637475397</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>5.7883374475500702</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>5.7082043904962498</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>5.6144136809769902</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>5.5256936776569301</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>5.3835194730617904</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.2189926932794002</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.1767006727176001</c:v>
+                  <c:v>5.5101642502389296</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11758,51 +11533,6 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>368.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>368.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>368.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>368.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>369.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>369.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>369.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>369.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>369.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>370.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>370.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>370.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>370.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>370.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>371.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>371.39999999999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11859,178 +11589,133 @@
                   <c:v>4.4264075542562802</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.6563626323753802</c:v>
+                  <c:v>2.8531002316127001</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.6789998652238398</c:v>
+                  <c:v>2.8824543798668101</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>2.7020347861968199</c:v>
+                  <c:v>2.91213927462955</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.72540193146085</c:v>
+                  <c:v>2.9423658895290199</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.7489993608392398</c:v>
+                  <c:v>2.97335045770313</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>2.7730144403683799</c:v>
+                  <c:v>3.0047089993527498</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.79737648471309</c:v>
+                  <c:v>3.0366480477145501</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>2.8219815775772101</c:v>
+                  <c:v>3.06938835049734</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.8470395677946398</c:v>
+                  <c:v>3.1025302345000401</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.8724556087081199</c:v>
+                  <c:v>3.1362624263021202</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.8981154434937402</c:v>
+                  <c:v>3.1706156802835901</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.9242663966509999</c:v>
+                  <c:v>3.2056011295691</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>2.9506652454842599</c:v>
+                  <c:v>3.24123099886905</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>2.9775727572095398</c:v>
+                  <c:v>3.2775765627748501</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.00472762254245</c:v>
+                  <c:v>3.3142994248016402</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.03242028518746</c:v>
+                  <c:v>3.3519458315863702</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0603765933872298</c:v>
+                  <c:v>3.3903018857585399</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>3.0888913712488701</c:v>
+                  <c:v>3.4292123098740999</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>3.11767251432993</c:v>
+                  <c:v>3.46905176295492</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>3.1470352401498198</c:v>
+                  <c:v>3.5094150983626702</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1766798277811499</c:v>
+                  <c:v>3.5506792187559699</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.2067775022090101</c:v>
+                  <c:v>3.5926997823234199</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.2373386829415698</c:v>
+                  <c:v>3.6353685629694699</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.2685488238789699</c:v>
+                  <c:v>3.6793127638147198</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.3000717155730999</c:v>
+                  <c:v>3.7239086094375602</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>3.3321013288048702</c:v>
+                  <c:v>3.76969783538929</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>3.3646548282586002</c:v>
+                  <c:v>3.8162745603866499</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>3.3977296008513602</c:v>
+                  <c:v>3.8643092047473102</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>3.4313901570629701</c:v>
+                  <c:v>3.91327673162627</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>3.4654524094832899</c:v>
+                  <c:v>3.9639220053655402</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>3.50031049286109</c:v>
+                  <c:v>4.0160633169199</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>3.5356896644051399</c:v>
+                  <c:v>4.0695741153676801</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>3.5718766570333802</c:v>
+                  <c:v>4.1253983256757802</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>3.6085955970210599</c:v>
+                  <c:v>4.1831517733499304</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>3.6460762289934201</c:v>
+                  <c:v>4.2437064262652697</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.6843655108036999</c:v>
+                  <c:v>4.30711417948143</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.7236478087345599</c:v>
+                  <c:v>4.3743908476388302</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>3.7635569050858999</c:v>
+                  <c:v>4.44648047249082</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>3.80447931122325</c:v>
+                  <c:v>4.5248235803186203</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>3.84649617019529</c:v>
+                  <c:v>4.6111301540093601</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>3.8896589765555301</c:v>
+                  <c:v>4.7097269013225596</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>3.93402918314922</c:v>
+                  <c:v>4.8005269780342301</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>3.97991302157924</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>4.02723884162</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>4.07629253628272</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>4.1272113050055204</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>4.1804769580021004</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>4.2363421539307202</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>4.2953649712256299</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>4.3585978267418799</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>4.4264075542626404</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>4.5005994716257698</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>4.5835983449190403</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>4.6816306404680699</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>4.7692325677298504</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>4.9164465213469697</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>5.0798197261805598</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>5.1187358618182</c:v>
+                  <c:v>4.9441771534810304</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12199,51 +11884,6 @@
                 </c:pt>
                 <c:pt idx="52">
                   <c:v>368.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>368.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>368.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>368.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>369.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>369.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>369.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>369.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>369.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>370.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>370.39999999999901</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>370.599999999999</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>370.79999999999899</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>370.99999999999898</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>371.19999999999902</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>371.39999999999901</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -33162,16 +32802,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>495300</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>666750</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
-      <xdr:row>27</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>219075</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -33567,39 +33207,39 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_V_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="propane_Pp_V_1" connectionId="9" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_Tp_L" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="propane_Pp_L" connectionId="8" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_L_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_Tp_L_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_Tp_V" connectionId="7" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_L" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_V_2" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_Tp_L" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_L_1" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
 <file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="octane_Tp_L_1" connectionId="6" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_V_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_V_3" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="methane_Pp_L" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -33903,7 +33543,7 @@
   <dimension ref="A1:X109"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -34294,16 +33934,16 @@
         <v>360</v>
       </c>
       <c r="B12">
-        <v>7.4831424502627097</v>
+        <v>7.3018891515019302</v>
       </c>
       <c r="C12">
-        <v>34.642891981919497</v>
+        <v>34.842352620883197</v>
       </c>
       <c r="D12">
-        <v>2.6563626323753802</v>
+        <v>2.8531002316127001</v>
       </c>
       <c r="E12">
-        <v>34.645889337403403</v>
+        <v>34.845015308570296</v>
       </c>
       <c r="P12">
         <v>7.66</v>
@@ -34329,16 +33969,16 @@
         <v>360.19999999999902</v>
       </c>
       <c r="B13">
-        <v>7.4611222799053003</v>
+        <v>7.2766672008740603</v>
       </c>
       <c r="C13">
-        <v>34.784199883701902</v>
+        <v>34.987904494824903</v>
       </c>
       <c r="D13">
-        <v>2.6789998652238398</v>
+        <v>2.8824543798668101</v>
       </c>
       <c r="E13">
-        <v>34.786376833659403</v>
+        <v>34.991311900615102</v>
       </c>
       <c r="P13">
         <v>7.8</v>
@@ -34364,16 +34004,16 @@
         <v>360.39999999999901</v>
       </c>
       <c r="B14">
-        <v>7.4388143614602802</v>
+        <v>7.2512626345506597</v>
       </c>
       <c r="C14">
-        <v>34.925265348824603</v>
+        <v>35.134884796496003</v>
       </c>
       <c r="D14">
-        <v>2.7020347861968199</v>
+        <v>2.91213927462955</v>
       </c>
       <c r="E14">
-        <v>34.927730029337397</v>
+        <v>35.137899592907701</v>
       </c>
       <c r="P14">
         <v>7.95</v>
@@ -34399,16 +34039,16 @@
         <v>360.599999999999</v>
       </c>
       <c r="B15">
-        <v>7.41630016041786</v>
+        <v>7.2255672912393996</v>
       </c>
       <c r="C15">
-        <v>35.066838561414599</v>
+        <v>35.2826385485956</v>
       </c>
       <c r="D15">
-        <v>2.72540193146085</v>
+        <v>2.9423658895290199</v>
       </c>
       <c r="E15">
-        <v>35.0697295457013</v>
+        <v>35.2852647153235</v>
       </c>
       <c r="P15">
         <v>8.09</v>
@@ -34434,16 +34074,16 @@
         <v>360.79999999999899</v>
       </c>
       <c r="B16">
-        <v>7.3936968588212304</v>
+        <v>7.1994684442101198</v>
       </c>
       <c r="C16">
-        <v>35.209888874959397</v>
+        <v>35.430556350401503</v>
       </c>
       <c r="D16">
-        <v>2.7489993608392398</v>
+        <v>2.97335045770313</v>
       </c>
       <c r="E16">
-        <v>35.2120641713786</v>
+        <v>35.433863707544603</v>
       </c>
       <c r="P16">
         <v>8.24</v>
@@ -34469,16 +34109,16 @@
         <v>360.99999999999898</v>
       </c>
       <c r="B17">
-        <v>7.3707901607294604</v>
+        <v>7.1731400810556103</v>
       </c>
       <c r="C17">
-        <v>35.352761955459599</v>
+        <v>35.579778826172401</v>
       </c>
       <c r="D17">
-        <v>2.7730144403683799</v>
+        <v>3.0047089993527498</v>
       </c>
       <c r="E17">
-        <v>35.3552753934949</v>
+        <v>35.582836097645497</v>
       </c>
       <c r="P17">
         <v>8.3800000000000008</v>
@@ -34504,16 +34144,16 @@
         <v>361.19999999999902</v>
       </c>
       <c r="B18">
-        <v>7.3476746441518497</v>
+        <v>7.1464790066373496</v>
       </c>
       <c r="C18">
-        <v>35.496265793378299</v>
+        <v>35.729750281573203</v>
       </c>
       <c r="D18">
-        <v>2.79737648471309</v>
+        <v>3.0366480477145501</v>
       </c>
       <c r="E18">
-        <v>35.499138819707902</v>
+        <v>35.732625826480302</v>
       </c>
       <c r="P18">
         <v>8.5299999999999994</v>
@@ -34539,16 +34179,16 @@
         <v>361.39999999999901</v>
       </c>
       <c r="B19">
-        <v>7.3244412252413902</v>
+        <v>7.1193850451695502</v>
       </c>
       <c r="C19">
-        <v>35.641112056516498</v>
+        <v>35.880002453428098</v>
       </c>
       <c r="D19">
-        <v>2.8219815775772101</v>
+        <v>3.06938835049734</v>
       </c>
       <c r="E19">
-        <v>35.643351734063103</v>
+        <v>35.8836662525881</v>
       </c>
       <c r="P19">
         <v>8.67</v>
@@ -34574,16 +34214,16 @@
         <v>361.599999999999</v>
       </c>
       <c r="B20">
-        <v>7.3008816821148601</v>
+        <v>7.0920333311784196</v>
       </c>
       <c r="C20">
-        <v>35.785811733904502</v>
+        <v>36.031590582370498</v>
       </c>
       <c r="D20">
-        <v>2.8470395677946398</v>
+        <v>3.1025302345000401</v>
       </c>
       <c r="E20">
-        <v>35.788489989048003</v>
+        <v>36.035120585260998</v>
       </c>
       <c r="P20">
         <v>8.82</v>
@@ -34609,16 +34249,16 @@
         <v>361.79999999999899</v>
       </c>
       <c r="B21">
-        <v>7.27709836821181</v>
+        <v>7.0642999904731596</v>
       </c>
       <c r="C21">
-        <v>35.931183106709703</v>
+        <v>36.183911866677398</v>
       </c>
       <c r="D21">
-        <v>2.8724556087081199</v>
+        <v>3.1362624263021202</v>
       </c>
       <c r="E21">
-        <v>35.9342722821672</v>
+        <v>36.187367381036204</v>
       </c>
       <c r="P21">
         <v>8.9600000000000009</v>
@@ -34644,16 +34284,16 @@
         <v>361.99999999999898</v>
       </c>
       <c r="B22">
-        <v>7.2531813195828603</v>
+        <v>7.0361768613322502</v>
       </c>
       <c r="C22">
-        <v>36.077885756664401</v>
+        <v>36.337016036260898</v>
       </c>
       <c r="D22">
-        <v>2.8981154434937402</v>
+        <v>3.1706156802835901</v>
       </c>
       <c r="E22">
-        <v>36.0803820558084</v>
+        <v>36.340452021841401</v>
       </c>
       <c r="P22">
         <v>9.11</v>
@@ -34679,16 +34319,16 @@
         <v>362.19999999999902</v>
       </c>
       <c r="B23">
-        <v>7.2289090372456997</v>
+        <v>7.0076464721156997</v>
       </c>
       <c r="C23">
-        <v>36.224453189127303</v>
+        <v>36.490910092770299</v>
       </c>
       <c r="D23">
-        <v>2.9242663966509999</v>
+        <v>3.2056011295691</v>
       </c>
       <c r="E23">
-        <v>36.227466030799498</v>
+        <v>36.494378735286602</v>
       </c>
       <c r="P23">
         <v>9.25</v>
@@ -34714,16 +34354,16 @@
         <v>362.39999999999901</v>
       </c>
       <c r="B24">
-        <v>7.2044943211291796</v>
+        <v>6.9786894935616903</v>
       </c>
       <c r="C24">
-        <v>36.372370647484203</v>
+        <v>36.645598689250903</v>
       </c>
       <c r="D24">
-        <v>2.9506652454842599</v>
+        <v>3.24123099886905</v>
       </c>
       <c r="E24">
-        <v>36.374872127760497</v>
+        <v>36.649152049319603</v>
       </c>
       <c r="P24">
         <v>9.39</v>
@@ -34749,16 +34389,16 @@
         <v>362.599999999999</v>
       </c>
       <c r="B25">
-        <v>7.1797101657913496</v>
+        <v>6.94927443655574</v>
       </c>
       <c r="C25">
-        <v>36.520211105239099</v>
+        <v>36.8010385713213</v>
       </c>
       <c r="D25">
-        <v>2.9775727572095398</v>
+        <v>3.2775765627748501</v>
       </c>
       <c r="E25">
-        <v>36.523257237233501</v>
+        <v>36.804877522812397</v>
       </c>
       <c r="P25">
         <v>9.5299999999999994</v>
@@ -34784,16 +34424,16 @@
         <v>362.79999999999899</v>
       </c>
       <c r="B26">
-        <v>7.1547782843857899</v>
+        <v>6.9194854421776597</v>
       </c>
       <c r="C26">
-        <v>36.669444275542602</v>
+        <v>36.957695757109299</v>
       </c>
       <c r="D26">
-        <v>3.00472762254245</v>
+        <v>3.3142994248016402</v>
       </c>
       <c r="E26">
-        <v>36.671946578979203</v>
+        <v>36.960951355264498</v>
       </c>
       <c r="P26">
         <v>9.67</v>
@@ -34819,16 +34459,16 @@
         <v>362.99999999999898</v>
       </c>
       <c r="B27">
-        <v>7.1294471958867396</v>
+        <v>6.8891167800800996</v>
       </c>
       <c r="C27">
-        <v>36.8185719294652</v>
+        <v>37.1147844590392</v>
       </c>
       <c r="D27">
-        <v>3.03242028518746</v>
+        <v>3.3519458315863702</v>
       </c>
       <c r="E27">
-        <v>36.821644025351901</v>
+        <v>37.118294283752597</v>
       </c>
       <c r="P27">
         <v>9.81</v>
@@ -34854,16 +34494,16 @@
         <v>363.19999999999902</v>
       </c>
       <c r="B28">
-        <v>7.1039347709624598</v>
+        <v>6.8582230834512101</v>
       </c>
       <c r="C28">
-        <v>36.968975569694699</v>
+        <v>37.272672366635497</v>
       </c>
       <c r="D28">
-        <v>3.0603765933872298</v>
+        <v>3.3903018857585399</v>
       </c>
       <c r="E28">
-        <v>36.971666514505799</v>
+        <v>37.276503998255897</v>
       </c>
       <c r="P28">
         <v>9.94</v>
@@ -34889,16 +34529,16 @@
         <v>363.39999999999901</v>
       </c>
       <c r="B29">
-        <v>7.0780099392793696</v>
+        <v>6.82685144210192</v>
       </c>
       <c r="C29">
-        <v>37.1193672660972</v>
+        <v>37.431653607261602</v>
       </c>
       <c r="D29">
-        <v>3.0888913712488701</v>
+        <v>3.4292123098740999</v>
       </c>
       <c r="E29">
-        <v>37.122697602738803</v>
+        <v>37.435308216641403</v>
       </c>
       <c r="P29">
         <v>10.08</v>
@@ -34924,16 +34564,16 @@
         <v>363.599999999999</v>
       </c>
       <c r="B30">
-        <v>7.0518882533204499</v>
+        <v>6.7948152129236501</v>
       </c>
       <c r="C30">
-        <v>37.271042590135202</v>
+        <v>37.591141466962597</v>
       </c>
       <c r="D30">
-        <v>3.11767251432993</v>
+        <v>3.46905176295492</v>
       </c>
       <c r="E30">
-        <v>37.274038150082802</v>
+        <v>37.595265087267002</v>
       </c>
       <c r="P30">
         <v>10.220000000000001</v>
@@ -34959,16 +34599,16 @@
         <v>363.79999999999899</v>
       </c>
       <c r="B31">
-        <v>7.0253397060208798</v>
+        <v>6.76224572120225</v>
       </c>
       <c r="C31">
-        <v>37.4227972824131</v>
+        <v>37.751754258756499</v>
       </c>
       <c r="D31">
-        <v>3.1470352401498198</v>
+        <v>3.5094150983626702</v>
       </c>
       <c r="E31">
-        <v>37.426388292401697</v>
+        <v>37.755717475365202</v>
       </c>
       <c r="P31">
         <v>10.35</v>
@@ -34994,16 +34634,16 @@
         <v>363.99999999999898</v>
       </c>
       <c r="B32">
-        <v>6.9985578180577601</v>
+        <v>6.7289937059384597</v>
       </c>
       <c r="C32">
-        <v>37.575742591242097</v>
+        <v>37.9130954060061</v>
       </c>
       <c r="D32">
-        <v>3.1766798277811499</v>
+        <v>3.5506792187559699</v>
       </c>
       <c r="E32">
-        <v>37.579056274961196</v>
+        <v>37.917193404168003</v>
       </c>
       <c r="P32">
         <v>10.49</v>
@@ -35029,16 +34669,16 @@
         <v>364.19999999999902</v>
       </c>
       <c r="B33">
-        <v>6.9714204339209003</v>
+        <v>6.6950438339079597</v>
       </c>
       <c r="C33">
-        <v>37.729294141154803</v>
+        <v>38.075269858279697</v>
       </c>
       <c r="D33">
-        <v>3.2067775022090101</v>
+        <v>3.5926997823234199</v>
       </c>
       <c r="E33">
-        <v>37.732406006891303</v>
+        <v>38.079432357345098</v>
       </c>
       <c r="P33">
         <v>10.64</v>
@@ -35064,16 +34704,16 @@
         <v>364.39999999999901</v>
       </c>
       <c r="B34">
-        <v>6.9439131958592304</v>
+        <v>6.6604192436680902</v>
       </c>
       <c r="C34">
-        <v>37.8834615702809</v>
+        <v>38.238492347002399</v>
       </c>
       <c r="D34">
-        <v>3.2373386829415698</v>
+        <v>3.6353685629694699</v>
       </c>
       <c r="E34">
-        <v>37.886435001704797</v>
+        <v>38.242247831969699</v>
       </c>
       <c r="P34">
         <v>10.78</v>
@@ -35099,16 +34739,16 @@
         <v>364.599999999999</v>
       </c>
       <c r="B35">
-        <v>6.9159019831246802</v>
+        <v>6.6248628520981301</v>
       </c>
       <c r="C35">
-        <v>38.037703004000797</v>
+        <v>38.402167553409697</v>
       </c>
       <c r="D35">
-        <v>3.2685488238789699</v>
+        <v>3.6793127638147198</v>
       </c>
       <c r="E35">
-        <v>38.041493153379101</v>
+        <v>38.406412639390297</v>
       </c>
       <c r="P35">
         <v>10.93</v>
@@ -35134,16 +34774,16 @@
         <v>364.79999999999899</v>
       </c>
       <c r="B36">
-        <v>6.8876090933653904</v>
+        <v>6.58852417074442</v>
       </c>
       <c r="C36">
-        <v>38.193151274937797</v>
+        <v>38.5669154842643</v>
       </c>
       <c r="D36">
-        <v>3.3000717155730999</v>
+        <v>3.7239086094375602</v>
       </c>
       <c r="E36">
-        <v>38.196863220224401</v>
+        <v>38.571038054832798</v>
       </c>
       <c r="P36">
         <v>11.07</v>
@@ -35169,16 +34809,16 @@
         <v>364.99999999999898</v>
       </c>
       <c r="B37">
-        <v>6.8588917375556901</v>
+        <v>6.55119306636694</v>
       </c>
       <c r="C37">
-        <v>38.349218575694401</v>
+        <v>38.732354549600601</v>
       </c>
       <c r="D37">
-        <v>3.3321013288048702</v>
+        <v>3.76969783538929</v>
       </c>
       <c r="E37">
-        <v>38.352915402140503</v>
+        <v>38.736731430078102</v>
       </c>
       <c r="P37">
         <v>11.22</v>
@@ -35204,16 +34844,16 @@
         <v>365.19999999999902</v>
       </c>
       <c r="B38">
-        <v>6.8297287323044502</v>
+        <v>6.5129203956428299</v>
       </c>
       <c r="C38">
-        <v>38.505906597864801</v>
+        <v>38.898817671040597</v>
       </c>
       <c r="D38">
-        <v>3.3646548282586002</v>
+        <v>3.8162745603866499</v>
       </c>
       <c r="E38">
-        <v>38.5096496517994</v>
+        <v>38.9029207134651</v>
       </c>
       <c r="P38">
         <v>11.36</v>
@@ -35239,16 +34879,16 @@
         <v>365.39999999999901</v>
       </c>
       <c r="B39">
-        <v>6.8001270657856798</v>
+        <v>6.47339369910532</v>
       </c>
       <c r="C39">
-        <v>38.663338174684498</v>
+        <v>39.0657974707675</v>
       </c>
       <c r="D39">
-        <v>3.3977296008513602</v>
+        <v>3.8643092047473102</v>
       </c>
       <c r="E39">
-        <v>38.667026038769897</v>
+        <v>39.070276489066103</v>
       </c>
       <c r="P39">
         <v>11.51</v>
@@ -35274,16 +34914,16 @@
         <v>365.599999999999</v>
       </c>
       <c r="B40">
-        <v>6.7700018202915802</v>
+        <v>6.43276529681975</v>
       </c>
       <c r="C40">
-        <v>38.821272323558503</v>
+        <v>39.233884301274202</v>
       </c>
       <c r="D40">
-        <v>3.4313901570629701</v>
+        <v>3.91327673162627</v>
       </c>
       <c r="E40">
-        <v>38.825124636515802</v>
+        <v>39.238103862201399</v>
       </c>
       <c r="P40">
         <v>11.65</v>
@@ -35309,16 +34949,16 @@
         <v>365.79999999999899</v>
       </c>
       <c r="B41">
-        <v>6.7394769323194703</v>
+        <v>6.3906744816543402</v>
       </c>
       <c r="C41">
-        <v>38.980281154274998</v>
+        <v>39.402592713501903</v>
       </c>
       <c r="D41">
-        <v>3.4654524094832899</v>
+        <v>3.9639220053655402</v>
       </c>
       <c r="E41">
-        <v>38.983581340417302</v>
+        <v>39.407053578167101</v>
       </c>
       <c r="P41">
         <v>11.8</v>
@@ -35344,16 +34984,16 @@
         <v>365.99999999999898</v>
       </c>
       <c r="B42">
-        <v>6.7082793330174697</v>
+        <v>6.3470732133511198</v>
       </c>
       <c r="C42">
-        <v>39.139455669267797</v>
+        <v>39.572149149139697</v>
       </c>
       <c r="D42">
-        <v>3.50031049286109</v>
+        <v>4.0160633169199</v>
       </c>
       <c r="E42">
-        <v>39.143042722784301</v>
+        <v>39.576767992627303</v>
       </c>
       <c r="P42">
         <v>11.94</v>
@@ -35379,16 +35019,16 @@
         <v>366.19999999999902</v>
       </c>
       <c r="B43">
-        <v>6.6765942738238504</v>
+        <v>6.3017796878727799</v>
       </c>
       <c r="C43">
-        <v>39.299589815164197</v>
+        <v>39.742558688364497</v>
       </c>
       <c r="D43">
-        <v>3.5356896644051399</v>
+        <v>4.0695741153676801</v>
       </c>
       <c r="E43">
-        <v>39.302983085392</v>
+        <v>39.746980567877699</v>
       </c>
       <c r="P43">
         <v>12.09</v>
@@ -35414,16 +35054,16 @@
         <v>366.39999999999901</v>
       </c>
       <c r="B44">
-        <v>6.6441820109603702</v>
+        <v>6.2544678428308504</v>
       </c>
       <c r="C44">
-        <v>39.459989326798699</v>
+        <v>39.913676150553897</v>
       </c>
       <c r="D44">
-        <v>3.5718766570333802</v>
+        <v>4.1253983256757802</v>
       </c>
       <c r="E44">
-        <v>39.463821025764197</v>
+        <v>39.918315466547902</v>
       </c>
       <c r="P44">
         <v>12.23</v>
@@ -35449,16 +35089,16 @@
         <v>366.599999999999</v>
       </c>
       <c r="B45">
-        <v>6.6112217940153597</v>
+        <v>6.2049688977114403</v>
       </c>
       <c r="C45">
-        <v>39.621377507594303</v>
+        <v>40.085682094038503</v>
       </c>
       <c r="D45">
-        <v>3.6085955970210599</v>
+        <v>4.1831517733499304</v>
       </c>
       <c r="E45">
-        <v>39.625054928453999</v>
+        <v>40.090203719673703</v>
       </c>
       <c r="P45">
         <v>12.38</v>
@@ -35484,16 +35124,16 @@
         <v>366.79999999999899</v>
       </c>
       <c r="B46">
-        <v>6.5775455297792398</v>
+        <v>6.1526786449464304</v>
       </c>
       <c r="C46">
-        <v>39.783348209641701</v>
+        <v>40.258288120218502</v>
       </c>
       <c r="D46">
-        <v>3.6460762289934201</v>
+        <v>4.2437064262652697</v>
       </c>
       <c r="E46">
-        <v>39.786988246620702</v>
+        <v>40.263029947619202</v>
       </c>
       <c r="P46">
         <v>12.53</v>
@@ -35519,16 +35159,16 @@
         <v>366.99999999999898</v>
       </c>
       <c r="B47">
-        <v>6.5431011109783697</v>
+        <v>6.0973673724428501</v>
       </c>
       <c r="C47">
-        <v>39.945904411970801</v>
+        <v>40.431814431181699</v>
       </c>
       <c r="D47">
-        <v>3.6843655108036999</v>
+        <v>4.30711417948143</v>
       </c>
       <c r="E47">
-        <v>39.949616136718397</v>
+        <v>40.436481331258499</v>
       </c>
       <c r="P47">
         <v>12.67</v>
@@ -35554,16 +35194,16 @@
         <v>367.19999999999902</v>
       </c>
       <c r="B48">
-        <v>6.5077401965147601</v>
+        <v>6.03810345559108</v>
       </c>
       <c r="C48">
-        <v>40.108815865754202</v>
+        <v>40.605990010074798</v>
       </c>
       <c r="D48">
-        <v>3.7236478087345599</v>
+        <v>4.3743908476388302</v>
       </c>
       <c r="E48">
-        <v>40.113112293822901</v>
+        <v>40.610783840922203</v>
       </c>
       <c r="P48">
         <v>12.82</v>
@@ -35583,16 +35223,16 @@
         <v>367.39999999999901</v>
       </c>
       <c r="B49">
-        <v>6.4716884292177204</v>
+        <v>5.9742055756659802</v>
       </c>
       <c r="C49">
-        <v>40.272843546997301</v>
+        <v>40.781058709310898</v>
       </c>
       <c r="D49">
-        <v>3.7635569050858999</v>
+        <v>4.44648047249082</v>
       </c>
       <c r="E49">
-        <v>40.2768871016278</v>
+        <v>40.785903072507899</v>
       </c>
       <c r="P49">
         <v>12.96</v>
@@ -35612,16 +35252,16 @@
         <v>367.599999999999</v>
       </c>
       <c r="B50">
-        <v>6.4346555663204601</v>
+        <v>5.90414454234367</v>
       </c>
       <c r="C50">
-        <v>40.437406489114998</v>
+        <v>40.956904102251102</v>
       </c>
       <c r="D50">
-        <v>3.80447931122325</v>
+        <v>4.5248235803186203</v>
       </c>
       <c r="E50">
-        <v>40.441381504629703</v>
+        <v>40.961810241869102</v>
       </c>
       <c r="P50">
         <v>13.11</v>
@@ -35641,16 +35281,16 @@
         <v>367.79999999999899</v>
       </c>
       <c r="B51">
-        <v>6.3965538532516897</v>
+        <v>5.8252621445605497</v>
       </c>
       <c r="C51">
-        <v>40.602513182169197</v>
+        <v>41.133366215811698</v>
       </c>
       <c r="D51">
-        <v>3.84649617019529</v>
+        <v>4.6111301540093601</v>
       </c>
       <c r="E51">
-        <v>40.606584340992796</v>
+        <v>41.138274168016103</v>
       </c>
       <c r="P51">
         <v>13.25</v>
@@ -35670,16 +35310,16 @@
         <v>367.99999999999898</v>
       </c>
       <c r="B52">
-        <v>6.3573667733563202</v>
+        <v>5.7329821766848204</v>
       </c>
       <c r="C52">
-        <v>40.768344322168197</v>
+        <v>41.310479629077903</v>
       </c>
       <c r="D52">
-        <v>3.8896589765555301</v>
+        <v>4.7097269013225596</v>
       </c>
       <c r="E52">
-        <v>40.772434626252199</v>
+        <v>41.3154075510176</v>
       </c>
       <c r="P52">
         <v>13.4</v>
@@ -35699,16 +35339,16 @@
         <v>368.19999999999902</v>
       </c>
       <c r="B53">
-        <v>6.3169155565285697</v>
+        <v>5.6322921702051296</v>
       </c>
       <c r="C53">
-        <v>40.934759430510603</v>
+        <v>41.491122903159997</v>
       </c>
       <c r="D53">
-        <v>3.93402918314922</v>
+        <v>4.8005269780342301</v>
       </c>
       <c r="E53">
-        <v>40.938873788102299</v>
+        <v>41.488676211309603</v>
       </c>
       <c r="P53">
         <v>13.55</v>
@@ -35728,16 +35368,16 @@
         <v>368.39999999999901</v>
       </c>
       <c r="B54">
-        <v>6.2749825629684697</v>
+        <v>5.5101642502389296</v>
       </c>
       <c r="C54">
-        <v>41.101624535925801</v>
+        <v>41.6726240396601</v>
       </c>
       <c r="D54">
-        <v>3.97991302157924</v>
+        <v>4.9441771534810304</v>
       </c>
       <c r="E54">
-        <v>41.106082816166101</v>
+        <v>41.667632393692898</v>
       </c>
       <c r="P54">
         <v>13.69</v>
@@ -35753,21 +35393,6 @@
       </c>
     </row>
     <row r="55" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A55">
-        <v>368.599999999999</v>
-      </c>
-      <c r="B55">
-        <v>6.23156863249437</v>
-      </c>
-      <c r="C55">
-        <v>41.269240846022903</v>
-      </c>
-      <c r="D55">
-        <v>4.02723884162</v>
-      </c>
-      <c r="E55">
-        <v>41.273812097923503</v>
-      </c>
       <c r="P55">
         <v>13.84</v>
       </c>
@@ -35782,21 +35407,6 @@
       </c>
     </row>
     <row r="56" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A56">
-        <v>368.79999999999899</v>
-      </c>
-      <c r="B56">
-        <v>6.1865116347403202</v>
-      </c>
-      <c r="C56">
-        <v>41.437629944779196</v>
-      </c>
-      <c r="D56">
-        <v>4.07629253628272</v>
-      </c>
-      <c r="E56">
-        <v>41.442158170747703</v>
-      </c>
       <c r="P56">
         <v>13.98</v>
       </c>
@@ -35811,21 +35421,6 @@
       </c>
     </row>
     <row r="57" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A57">
-        <v>368.99999999999898</v>
-      </c>
-      <c r="B57">
-        <v>6.1393419397654503</v>
-      </c>
-      <c r="C57">
-        <v>41.606451722751601</v>
-      </c>
-      <c r="D57">
-        <v>4.1272113050055204</v>
-      </c>
-      <c r="E57">
-        <v>41.611033233424301</v>
-      </c>
       <c r="P57">
         <v>14.13</v>
       </c>
@@ -35840,21 +35435,6 @@
       </c>
     </row>
     <row r="58" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A58">
-        <v>369.19999999999902</v>
-      </c>
-      <c r="B58">
-        <v>6.0900581556244102</v>
-      </c>
-      <c r="C58">
-        <v>41.776113552696302</v>
-      </c>
-      <c r="D58">
-        <v>4.1804769580021004</v>
-      </c>
-      <c r="E58">
-        <v>41.780590537770898</v>
-      </c>
       <c r="P58">
         <v>14.27</v>
       </c>
@@ -35869,21 +35449,6 @@
       </c>
     </row>
     <row r="59" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A59">
-        <v>369.39999999999901</v>
-      </c>
-      <c r="B59">
-        <v>6.0378291254429799</v>
-      </c>
-      <c r="C59">
-        <v>41.946084886906696</v>
-      </c>
-      <c r="D59">
-        <v>4.2363421539307202</v>
-      </c>
-      <c r="E59">
-        <v>41.950717442605701</v>
-      </c>
       <c r="P59">
         <v>14.42</v>
       </c>
@@ -35898,21 +35463,6 @@
       </c>
     </row>
     <row r="60" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A60">
-        <v>369.599999999999</v>
-      </c>
-      <c r="B60">
-        <v>5.98253987504809</v>
-      </c>
-      <c r="C60">
-        <v>42.116833187358097</v>
-      </c>
-      <c r="D60">
-        <v>4.2953649712256299</v>
-      </c>
-      <c r="E60">
-        <v>42.121449536862599</v>
-      </c>
       <c r="P60">
         <v>14.57</v>
       </c>
@@ -35927,21 +35477,6 @@
       </c>
     </row>
     <row r="61" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A61">
-        <v>369.79999999999899</v>
-      </c>
-      <c r="B61">
-        <v>5.9232941847193104</v>
-      </c>
-      <c r="C61">
-        <v>42.288155040503298</v>
-      </c>
-      <c r="D61">
-        <v>4.3585978267418799</v>
-      </c>
-      <c r="E61">
-        <v>42.2929730689198</v>
-      </c>
       <c r="P61">
         <v>14.71</v>
       </c>
@@ -35956,21 +35491,6 @@
       </c>
     </row>
     <row r="62" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A62">
-        <v>369.99999999999898</v>
-      </c>
-      <c r="B62">
-        <v>5.8591042637475397</v>
-      </c>
-      <c r="C62">
-        <v>42.4600827726075</v>
-      </c>
-      <c r="D62">
-        <v>4.4264075542626404</v>
-      </c>
-      <c r="E62">
-        <v>42.464911071649396</v>
-      </c>
       <c r="P62">
         <v>14.86</v>
       </c>
@@ -35985,21 +35505,6 @@
       </c>
     </row>
     <row r="63" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A63">
-        <v>370.19999999999902</v>
-      </c>
-      <c r="B63">
-        <v>5.7883374475500702</v>
-      </c>
-      <c r="C63">
-        <v>42.632579463731503</v>
-      </c>
-      <c r="D63">
-        <v>4.5005994716257698</v>
-      </c>
-      <c r="E63">
-        <v>42.637431668547499</v>
-      </c>
       <c r="P63">
         <v>15</v>
       </c>
@@ -36014,21 +35519,6 @@
       </c>
     </row>
     <row r="64" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A64">
-        <v>370.39999999999901</v>
-      </c>
-      <c r="B64">
-        <v>5.7082043904962498</v>
-      </c>
-      <c r="C64">
-        <v>42.805605187939598</v>
-      </c>
-      <c r="D64">
-        <v>4.5835983449190403</v>
-      </c>
-      <c r="E64">
-        <v>42.810497148708997</v>
-      </c>
       <c r="P64">
         <v>15.15</v>
       </c>
@@ -36042,22 +35532,7 @@
         <v>327.91</v>
       </c>
     </row>
-    <row r="65" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A65">
-        <v>370.599999999999</v>
-      </c>
-      <c r="B65">
-        <v>5.6144136809769902</v>
-      </c>
-      <c r="C65">
-        <v>42.979457979611098</v>
-      </c>
-      <c r="D65">
-        <v>4.6816306404680699</v>
-      </c>
-      <c r="E65">
-        <v>42.984416209589</v>
-      </c>
+    <row r="65" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P65">
         <v>15.3</v>
       </c>
@@ -36071,22 +35546,7 @@
         <v>319.57</v>
       </c>
     </row>
-    <row r="66" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A66">
-        <v>370.79999999999899</v>
-      </c>
-      <c r="B66">
-        <v>5.5256936776569301</v>
-      </c>
-      <c r="C66">
-        <v>43.158833678275698</v>
-      </c>
-      <c r="D66">
-        <v>4.7692325677298504</v>
-      </c>
-      <c r="E66">
-        <v>43.153859152428701</v>
-      </c>
+    <row r="66" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P66">
         <v>15.44</v>
       </c>
@@ -36100,22 +35560,7 @@
         <v>311.54000000000002</v>
       </c>
     </row>
-    <row r="67" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A67">
-        <v>370.99999999999898</v>
-      </c>
-      <c r="B67">
-        <v>5.3835194730617904</v>
-      </c>
-      <c r="C67">
-        <v>43.333919633036402</v>
-      </c>
-      <c r="D67">
-        <v>4.9164465213469697</v>
-      </c>
-      <c r="E67">
-        <v>43.328927528517802</v>
-      </c>
+    <row r="67" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P67">
         <v>15.59</v>
       </c>
@@ -36129,22 +35574,7 @@
         <v>303.35000000000002</v>
       </c>
     </row>
-    <row r="68" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A68">
-        <v>371.19999999999902</v>
-      </c>
-      <c r="B68">
-        <v>5.2189926932794002</v>
-      </c>
-      <c r="C68">
-        <v>43.509159976231501</v>
-      </c>
-      <c r="D68">
-        <v>5.0798197261805598</v>
-      </c>
-      <c r="E68">
-        <v>43.504161769781497</v>
-      </c>
+    <row r="68" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P68">
         <v>15.73</v>
       </c>
@@ -36158,22 +35588,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="69" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A69">
-        <v>371.39999999999901</v>
-      </c>
-      <c r="B69">
-        <v>5.1767006727176001</v>
-      </c>
-      <c r="C69">
-        <v>43.684236904605399</v>
-      </c>
-      <c r="D69">
-        <v>5.1187358618182</v>
-      </c>
-      <c r="E69">
-        <v>43.6792386926479</v>
-      </c>
+    <row r="69" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P69">
         <v>15.88</v>
       </c>
@@ -36187,7 +35602,7 @@
         <v>286.60000000000002</v>
       </c>
     </row>
-    <row r="70" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="70" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P70">
         <v>16.03</v>
       </c>
@@ -36201,7 +35616,7 @@
         <v>278.26</v>
       </c>
     </row>
-    <row r="71" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="71" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P71">
         <v>16.170000000000002</v>
       </c>
@@ -36215,7 +35630,7 @@
         <v>269.81</v>
       </c>
     </row>
-    <row r="72" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="72" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P72">
         <v>16.32</v>
       </c>
@@ -36229,7 +35644,7 @@
         <v>261.45999999999998</v>
       </c>
     </row>
-    <row r="73" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="73" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P73">
         <v>16.46</v>
       </c>
@@ -36243,7 +35658,7 @@
         <v>253.17</v>
       </c>
     </row>
-    <row r="74" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="74" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P74">
         <v>16.559999999999999</v>
       </c>
@@ -36257,7 +35672,7 @@
         <v>244.87</v>
       </c>
     </row>
-    <row r="75" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="75" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P75">
         <v>0</v>
       </c>
@@ -36271,7 +35686,7 @@
         <v>236.53</v>
       </c>
     </row>
-    <row r="76" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="76" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P76">
         <v>0.09</v>
       </c>
@@ -36285,7 +35700,7 @@
         <v>228.18</v>
       </c>
     </row>
-    <row r="77" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="77" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P77">
         <v>0.17</v>
       </c>
@@ -36299,7 +35714,7 @@
         <v>221.42</v>
       </c>
     </row>
-    <row r="78" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="78" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P78">
         <v>0.24</v>
       </c>
@@ -36307,7 +35722,7 @@
         <v>5.13</v>
       </c>
     </row>
-    <row r="79" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="79" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P79">
         <v>0.32</v>
       </c>
@@ -36315,7 +35730,7 @@
         <v>6.63</v>
       </c>
     </row>
-    <row r="80" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="80" spans="16:24" x14ac:dyDescent="0.25">
       <c r="P80">
         <v>0.39</v>
       </c>

</xml_diff>